<commit_message>
Updated URegina Website Experience
</commit_message>
<xml_diff>
--- a/Documentation/Lab 1.1 Prep & Analysis/URegina Website User Experience.xlsx
+++ b/Documentation/Lab 1.1 Prep & Analysis/URegina Website User Experience.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaya\Documents\ENSE-471-UI-Project-CodeBreakers\Documentation\Lab 1.1 Prep &amp; Analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="35">
   <si>
     <t>Utility</t>
   </si>
@@ -54,26 +59,83 @@
     <t>Current Students</t>
   </si>
   <si>
-    <t>Media</t>
-  </si>
-  <si>
     <t>Liked</t>
   </si>
   <si>
     <t>Disliked</t>
   </si>
   <si>
-    <t>Not Represented</t>
-  </si>
-  <si>
-    <t>Relevant Pages to Enhance</t>
+    <t>University of Regina</t>
+  </si>
+  <si>
+    <t>The different areas makes the overall website a little messy and lowers the quality</t>
+  </si>
+  <si>
+    <t>Disorganized layout which makes information hard to find</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> There are elements at the top, right, and left which makes navigation difficult. Though the information is grouped well</t>
+  </si>
+  <si>
+    <t>Low usability. Really lacking in important information e.g course schedules, tuition etc.</t>
+  </si>
+  <si>
+    <t>Can be confusing at times. Some links take you to a whole new page and the only way to go back is with the back button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The information and buttons that would be needed are there and behave predictably </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decent, the buttons work as expected but user can get lost sometimes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lack of information makes this less desirable </t>
+  </si>
+  <si>
+    <t>Website look and structure is consistent with the overall University's website (which is not good in the first place)</t>
+  </si>
+  <si>
+    <t>Really messy and bland. Lack of pictures and just blocks of text makes it really boring to navigate</t>
+  </si>
+  <si>
+    <t>Low desirability. There is nothing to lure users in and portrays UofR as a place that is outdated and not up to the standard</t>
+  </si>
+  <si>
+    <t>Fairly easy to get some good information about programs and the school. Some of the quick links are very useful</t>
+  </si>
+  <si>
+    <t>Grouping of elemets is good. The quick links and upcoming events tabs are very useful</t>
+  </si>
+  <si>
+    <t>Can be accessed easily but not a lot of information available. Some of the information is outdated and incomplete</t>
+  </si>
+  <si>
+    <t>Can be accessed easily and there is a fair bit of information available. Though some of the information is outdated and incomplete</t>
+  </si>
+  <si>
+    <t>Decent usability, some pages could use more information and more visual flair</t>
+  </si>
+  <si>
+    <t>Gets the job done but leaves a lot to be desired</t>
+  </si>
+  <si>
+    <t>Gets the job done. User can generally get most of the information they are looking for</t>
+  </si>
+  <si>
+    <t>Overall design is bland and uninspiring. Lots of white space on the pages. The website aspect ratio does not conform to the current industry standards</t>
+  </si>
+  <si>
+    <t>It can be hard to navigate sometimes and can sometimes get lost with no visible way of getting back. Some of the information is incompleted and outdated</t>
+  </si>
+  <si>
+    <t>Low desirability. Even though the information is there the website is unappealing and off putting. In need of an overhaul</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,8 +167,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,8 +196,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -143,8 +225,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -170,8 +261,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,8 +271,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -193,6 +293,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="25" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -209,6 +310,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -534,20 +643,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:K25"/>
+  <dimension ref="C1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:K22"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="11" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.296875" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
+    <col min="4" max="11" width="25.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11">
+    <row r="1" spans="3:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
@@ -564,58 +679,82 @@
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="3:11" ht="60" customHeight="1">
+    </row>
+    <row r="3" spans="3:9" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="3:11" ht="60" customHeight="1">
+      <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="3:11" ht="60" customHeight="1">
+      <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="7" spans="3:11">
+      <c r="D5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
@@ -632,58 +771,82 @@
         <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11" ht="60" customHeight="1">
+    </row>
+    <row r="8" spans="3:9" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="3:11" ht="60" customHeight="1">
+      <c r="D8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="3:11" ht="60" customHeight="1">
+      <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="12" spans="3:11">
+      <c r="D10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
@@ -700,58 +863,82 @@
         <v>5</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="3:11" ht="60" customHeight="1">
+    </row>
+    <row r="13" spans="3:9" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="3:11" ht="60" customHeight="1">
+      <c r="D13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="3:11" ht="60" customHeight="1">
+      <c r="D14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="17" spans="3:11">
+      <c r="D15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
         <v>8</v>
       </c>
@@ -768,128 +955,90 @@
         <v>5</v>
       </c>
       <c r="H17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="3:11" ht="60" customHeight="1">
+    </row>
+    <row r="18" spans="3:9" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="3:11" ht="60" customHeight="1">
+      <c r="D18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="3:11" ht="60" customHeight="1">
+      <c r="D19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="22" spans="3:11">
-      <c r="C22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J22" s="2" t="s">
+      <c r="D20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" ht="60" customHeight="1">
-      <c r="C23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="3:11" ht="60" customHeight="1">
-      <c r="C24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="3:11" ht="60" customHeight="1">
-      <c r="C25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-    </row>
+      <c r="F20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" ht="60" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="3:9" ht="60" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="3:9" ht="60" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>